<commit_message>
Added a gui that displays the data in graphs
</commit_message>
<xml_diff>
--- a/stock_data.xlsx
+++ b/stock_data.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="tesla" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="apple" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="nvidia" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Manchester" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="google" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="nike" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Tesla" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Apple" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Nvidia" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Manchester" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Google" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Nike" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -21,13 +21,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -46,12 +51,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -79,12 +99,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -452,36 +475,36 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E9:E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Price Text</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>Price Float</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>Note</t>
         </is>
@@ -495,20 +518,20 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>12:00:50</t>
+          <t>17:16:12</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>$298.26</t>
+          <t>$318.64</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>298.26</v>
+        <v>318.64</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Market Closed or Stale Data</t>
+          <t>Market Open</t>
         </is>
       </c>
     </row>
@@ -807,6 +830,131 @@
         <v>316.98</v>
       </c>
       <c r="E14" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>17:14:12</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>$318.13</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>318.13</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>17:17:46</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>$319.13</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>319.13</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>17:23:11</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>$319.04</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>319.04</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>17:30:21</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>$318.49</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>318.49</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>17:33:38</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>$318.60</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>318.6</v>
+      </c>
+      <c r="E19" t="inlineStr">
         <is>
           <t>Market Open</t>
         </is>
@@ -823,36 +971,36 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Price Text</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>Price Float</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>Note</t>
         </is>
@@ -866,20 +1014,20 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>12:13:43</t>
+          <t>17:16:20</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>$198.27</t>
+          <t>$208.33</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>198.27</v>
+        <v>208.33</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Market Closed or Stale Data</t>
+          <t>Market Open</t>
         </is>
       </c>
     </row>
@@ -1153,6 +1301,81 @@
         <v>210</v>
       </c>
       <c r="E13" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>17:18:04</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>$208.48</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>208.48</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>17:30:30</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>$208.66</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>208.66</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>17:34:03</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>$208.56</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>208.56</v>
+      </c>
+      <c r="E16" t="inlineStr">
         <is>
           <t>Market Open</t>
         </is>
@@ -1169,36 +1392,36 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E7:E8"/>
+      <selection activeCell="A15" sqref="A15:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Price Text</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>Price Float</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>Note</t>
         </is>
@@ -1212,20 +1435,20 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>12:13:53</t>
+          <t>17:16:27</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>$116.65</t>
+          <t>$121.83</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>116.65</v>
+        <v>121.83</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Market Closed or Stale Data</t>
+          <t>Market Open</t>
         </is>
       </c>
     </row>
@@ -1474,6 +1697,106 @@
         <v>120.98</v>
       </c>
       <c r="E12" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>17:18:11</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>$121.92</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>121.92</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>17:26:30</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>$122.32</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>122.32</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>17:30:38</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>$122.53</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>122.53</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>17:34:19</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>$122.63</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>122.63</v>
+      </c>
+      <c r="E16" t="inlineStr">
         <is>
           <t>Market Open</t>
         </is>
@@ -1490,36 +1813,36 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E7:E8"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Price Text</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>Price Float</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>Note</t>
         </is>
@@ -1533,20 +1856,20 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>12:14:02</t>
+          <t>17:16:34</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>$14.30</t>
+          <t>$14.49</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>14.3</v>
+        <v>14.49</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Market Closed or Stale Data</t>
+          <t>Market Open</t>
         </is>
       </c>
     </row>
@@ -1795,6 +2118,106 @@
         <v>14.4</v>
       </c>
       <c r="E12" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>17:18:20</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>$14.48</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>14.48</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>17:21:06</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>$14.60</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>14.6</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>17:30:54</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>$14.57</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>14.57</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>17:34:26</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>$14.57</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>14.57</v>
+      </c>
+      <c r="E16" t="inlineStr">
         <is>
           <t>Market Open</t>
         </is>
@@ -1811,36 +2234,36 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E7:E8"/>
+      <selection activeCell="A15" sqref="A15:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Price Text</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>Price Float</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>Note</t>
         </is>
@@ -1854,20 +2277,20 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>12:14:11</t>
+          <t>17:16:42</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>$152.75</t>
+          <t>$156.27</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>152.75</v>
+        <v>156.27</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Market Closed or Stale Data</t>
+          <t>Market Open</t>
         </is>
       </c>
     </row>
@@ -2116,6 +2539,106 @@
         <v>157.86</v>
       </c>
       <c r="E12" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>17:08:40</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>$156.53</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>156.53</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>17:18:27</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>$156.45</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>156.45</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>17:31:05</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>$156.82</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>156.82</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>17:34:34</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>$156.89</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>156.89</v>
+      </c>
+      <c r="E16" t="inlineStr">
         <is>
           <t>Market Open</t>
         </is>
@@ -2132,36 +2655,36 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Price Text</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>Price Float</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>Note</t>
         </is>
@@ -2175,20 +2698,20 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>12:14:20</t>
+          <t>17:16:49</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>$58.30</t>
+          <t>$62.08</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>58.3</v>
+        <v>62.08</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Market Closed or Stale Data</t>
+          <t>Market Open</t>
         </is>
       </c>
     </row>
@@ -2412,6 +2935,81 @@
         <v>62.9</v>
       </c>
       <c r="E11" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>17:18:34</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>$62.10</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>62.1</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>17:31:21</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>$62.41</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>62.41</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>17:35:08</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>$62.26</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>62.26</v>
+      </c>
+      <c r="E14" t="inlineStr">
         <is>
           <t>Market Open</t>
         </is>

</xml_diff>

<commit_message>
Add a exit button, logos for the companys and a button the extract and store data for all of the stocks.
</commit_message>
<xml_diff>
--- a/stock_data.xlsx
+++ b/stock_data.xlsx
@@ -1813,7 +1813,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
@@ -2218,6 +2218,31 @@
         <v>14.57</v>
       </c>
       <c r="E16" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>18:42:00</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>$14.61</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>14.61</v>
+      </c>
+      <c r="E17" t="inlineStr">
         <is>
           <t>Market Open</t>
         </is>
@@ -2234,7 +2259,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15:E15"/>
@@ -2639,6 +2664,31 @@
         <v>156.89</v>
       </c>
       <c r="E16" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>18:40:34</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>$158.26</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>158.26</v>
+      </c>
+      <c r="E17" t="inlineStr">
         <is>
           <t>Market Open</t>
         </is>

</xml_diff>

<commit_message>
Updated the layout og the app to be more user-friendly. Fixed some mistakes in the code.
</commit_message>
<xml_diff>
--- a/stock_data.xlsx
+++ b/stock_data.xlsx
@@ -475,7 +475,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18:E19"/>
@@ -955,6 +955,56 @@
         <v>318.6</v>
       </c>
       <c r="E19" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>19:08:39</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>$319.01</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>319.01</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>19:20:02</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>$318.16</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>318.16</v>
+      </c>
+      <c r="E21" t="inlineStr">
         <is>
           <t>Market Open</t>
         </is>
@@ -971,7 +1021,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J24" sqref="J24"/>
@@ -1376,6 +1426,56 @@
         <v>208.56</v>
       </c>
       <c r="E16" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>19:10:04</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>$210.86</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>210.86</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>19:20:09</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>$210.93</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>210.93</v>
+      </c>
+      <c r="E18" t="inlineStr">
         <is>
           <t>Market Open</t>
         </is>
@@ -1392,7 +1492,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15:E15"/>
@@ -1797,6 +1897,56 @@
         <v>122.63</v>
       </c>
       <c r="E16" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>19:07:58</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>$122.79</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>122.79</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>19:20:16</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>$122.80</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>122.8</v>
+      </c>
+      <c r="E18" t="inlineStr">
         <is>
           <t>Market Open</t>
         </is>
@@ -1813,7 +1963,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
@@ -2243,6 +2393,81 @@
         <v>14.61</v>
       </c>
       <c r="E17" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>19:19:36</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>$14.57</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>14.57</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>19:20:38</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>$14.57</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>14.57</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>19:20:53</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>$14.57</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>14.57</v>
+      </c>
+      <c r="E20" t="inlineStr">
         <is>
           <t>Market Open</t>
         </is>
@@ -2259,7 +2484,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15:E15"/>
@@ -2689,6 +2914,56 @@
         <v>158.26</v>
       </c>
       <c r="E17" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>18:52:45</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>$158.36</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>158.36</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>19:20:23</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>$158.38</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>158.38</v>
+      </c>
+      <c r="E19" t="inlineStr">
         <is>
           <t>Market Open</t>
         </is>
@@ -2705,7 +2980,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
@@ -3065,6 +3340,56 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>19:20:30</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>$62.44</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>62.44</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>19:21:05</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>$62.45</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>62.45</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Adjusted the graph and logo layout.
</commit_message>
<xml_diff>
--- a/stock_data.xlsx
+++ b/stock_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2424" yWindow="1764" windowWidth="17280" windowHeight="8880" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tesla" sheetId="1" state="visible" r:id="rId1"/>
@@ -21,18 +21,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <b val="1"/>
-      <sz val="11"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -51,27 +46,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -99,15 +79,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -475,36 +452,36 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:E19"/>
+      <selection activeCell="D8" sqref="D3:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Price Text</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Price Float</t>
         </is>
       </c>
-      <c r="E1" s="3" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Note</t>
         </is>
@@ -1007,6 +984,131 @@
       <c r="E21" t="inlineStr">
         <is>
           <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>21:04:16</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>$317.67</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>317.67</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>21:07:51</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>$317.81</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>317.81</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>21:09:54</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>$318.72</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>318.72</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>21:17:52</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>$318.60</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>318.6</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>21:23:11</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>$318.60</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>318.6</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
         </is>
       </c>
     </row>
@@ -1021,7 +1123,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J24" sqref="J24"/>
@@ -1030,27 +1132,27 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Price Text</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Price Float</t>
         </is>
       </c>
-      <c r="E1" s="3" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Note</t>
         </is>
@@ -1478,6 +1580,81 @@
       <c r="E18" t="inlineStr">
         <is>
           <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>19:25:52</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>$210.74</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>210.74</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>21:04:26</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>$210.08</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>210.08</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>21:07:59</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>$210.50</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>210.5</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
         </is>
       </c>
     </row>
@@ -1492,7 +1669,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15:E15"/>
@@ -1501,27 +1678,27 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Price Text</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Price Float</t>
         </is>
       </c>
-      <c r="E1" s="3" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Note</t>
         </is>
@@ -1949,6 +2126,106 @@
       <c r="E18" t="inlineStr">
         <is>
           <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>19:26:00</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>$122.60</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>122.6</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>21:04:34</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>$122.47</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>122.47</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>21:08:07</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>$122.88</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>122.88</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>21:21:33</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>$123.00</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>123</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
         </is>
       </c>
     </row>
@@ -1963,36 +2240,36 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Price Text</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Price Float</t>
         </is>
       </c>
-      <c r="E1" s="3" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Note</t>
         </is>
@@ -2470,6 +2747,106 @@
       <c r="E20" t="inlineStr">
         <is>
           <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>19:26:08</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>$14.58</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>14.58</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>21:04:42</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>$14.63</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>14.63</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>21:07:15</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>$14.62</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>14.62</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>21:08:33</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>$14.62</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>14.62</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
         </is>
       </c>
     </row>
@@ -2484,7 +2861,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15:E15"/>
@@ -2493,27 +2870,27 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Price Text</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Price Float</t>
         </is>
       </c>
-      <c r="E1" s="3" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Note</t>
         </is>
@@ -2966,6 +3343,156 @@
       <c r="E19" t="inlineStr">
         <is>
           <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>19:26:16</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>$158.40</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>158.4</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>21:04:50</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>$158.12</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>158.12</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>21:08:16</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>$158.24</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>158.24</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>21:16:24</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>$158.45</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>158.45</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>21:18:28</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>$158.45</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>158.45</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>21:20:36</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>$158.45</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>158.45</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
         </is>
       </c>
     </row>
@@ -2980,36 +3507,36 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Price Text</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Price Float</t>
         </is>
       </c>
-      <c r="E1" s="3" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Note</t>
         </is>
@@ -3387,6 +3914,131 @@
       <c r="E16" t="inlineStr">
         <is>
           <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>19:26:24</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>$62.29</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>62.29</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>19:27:21</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>$62.22</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>62.22</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Market Open</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>21:04:57</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>$62.41</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>62.41</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>21:06:26</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>$62.41</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>62.41</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>21:08:24</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>$62.46</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>62.46</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new graph options to the app.
</commit_message>
<xml_diff>
--- a/stock_data.xlsx
+++ b/stock_data.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D3:D8"/>
@@ -1107,6 +1107,131 @@
         <v>318.6</v>
       </c>
       <c r="E26" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-05-13</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>13:46:56</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>$318.38</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>318.38</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-05-13</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>13:50:49</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>$318.38</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>318.38</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-05-13</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>14:17:15</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>$318.38</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>318.38</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-05-13</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>14:18:11</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>$318.38</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>318.38</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-05-13</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>14:18:27</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>$318.38</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>318.38</v>
+      </c>
+      <c r="E31" t="inlineStr">
         <is>
           <t>Market Closed or Stale Data</t>
         </is>
@@ -1123,7 +1248,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J24" sqref="J24"/>
@@ -1653,6 +1778,31 @@
         <v>210.5</v>
       </c>
       <c r="E21" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-05-13</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>13:51:02</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>$210.79</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>210.79</v>
+      </c>
+      <c r="E22" t="inlineStr">
         <is>
           <t>Market Closed or Stale Data</t>
         </is>
@@ -1669,7 +1819,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15:E15"/>
@@ -2224,6 +2374,31 @@
         <v>123</v>
       </c>
       <c r="E22" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-05-13</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>13:51:10</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>$123.00</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>123</v>
+      </c>
+      <c r="E23" t="inlineStr">
         <is>
           <t>Market Closed or Stale Data</t>
         </is>
@@ -2240,7 +2415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
@@ -2845,6 +3020,181 @@
         <v>14.62</v>
       </c>
       <c r="E24" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>21:25:34</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>$14.61</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>14.61</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-05-13</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>13:51:36</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>$14.61</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>14.61</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-05-13</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>14:09:57</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>$14.61</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>14.61</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-05-13</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>14:10:17</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>$14.61</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>14.61</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-05-13</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>14:11:02</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>$14.61</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>14.61</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-05-13</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>14:11:36</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>$14.61</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>14.61</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-05-13</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>14:11:57</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>$14.61</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>14.61</v>
+      </c>
+      <c r="E31" t="inlineStr">
         <is>
           <t>Market Closed or Stale Data</t>
         </is>
@@ -2861,7 +3211,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15:E15"/>
@@ -3491,6 +3841,181 @@
         <v>158.45</v>
       </c>
       <c r="E25" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-05-13</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>13:51:19</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>$158.46</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>158.46</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-05-13</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>14:07:39</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>$158.46</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>158.46</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-05-13</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>14:08:08</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>$158.46</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>158.46</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-05-13</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>14:08:25</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>$158.46</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>158.46</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-05-13</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>14:08:40</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>$158.46</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>158.46</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-05-13</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>14:09:04</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>$158.46</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>158.46</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2025-05-13</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>14:09:29</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>$158.46</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>158.46</v>
+      </c>
+      <c r="E32" t="inlineStr">
         <is>
           <t>Market Closed or Stale Data</t>
         </is>
@@ -3507,7 +4032,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
@@ -4042,6 +4567,31 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-05-13</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>13:51:28</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>$62.58</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>62.58</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Market Closed or Stale Data</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>